<commit_message>
Source feito, limite de 2 tbm
</commit_message>
<xml_diff>
--- a/Resultados.xlsx
+++ b/Resultados.xlsx
@@ -437,7 +437,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D69"/>
+  <dimension ref="A1:E69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,6 +466,11 @@
           <t>Cor_CX 6200 Switch Series</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Fonte_CX 6200 Switch Series</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -486,6 +491,11 @@
           <t>yellow</t>
         </is>
       </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -498,12 +508,17 @@
       </c>
       <c r="C3" s="3" t="inlineStr">
         <is>
-          <t>12 portas SmartRate</t>
+          <t>12 ports SmartRate 100M/1G/2.5G/5G BaseT</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
           <t>green</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Page 25</t>
         </is>
       </c>
     </row>
@@ -518,12 +533,17 @@
       </c>
       <c r="C4" s="3" t="inlineStr">
         <is>
-          <t>4 portas 100M/1G/10G SFP+ (2x LRM</t>
+          <t>4x 100M/1G/10G SFP ports (2x LRM</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
           <t>green</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Page 25</t>
         </is>
       </c>
     </row>
@@ -538,12 +558,17 @@
       </c>
       <c r="C5" s="3" t="inlineStr">
         <is>
-          <t>2x LRM/MACSec 256)</t>
+          <t>4x 100M/1G/10G SFP ports (2x LRM/MACSec 256)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
           <t>green</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Page 25</t>
         </is>
       </c>
     </row>
@@ -566,6 +591,11 @@
           <t>green</t>
         </is>
       </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Page 25</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -586,6 +616,11 @@
           <t>green</t>
         </is>
       </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Page 25</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -606,6 +641,11 @@
           <t>green</t>
         </is>
       </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Page 25</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -626,6 +666,11 @@
           <t>green</t>
         </is>
       </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Page 25</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -646,6 +691,11 @@
           <t>green</t>
         </is>
       </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Page 25</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -666,6 +716,11 @@
           <t>green</t>
         </is>
       </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Page 25</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -686,6 +741,11 @@
           <t>green</t>
         </is>
       </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Page 25</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -706,6 +766,11 @@
           <t>green</t>
         </is>
       </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Page 25</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -718,12 +783,17 @@
       </c>
       <c r="C14" s="3" t="inlineStr">
         <is>
-          <t>8 members</t>
+          <t>Support for up to 8 switches (or members) in a stack via chain or ring topology</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
           <t>green</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Page 3</t>
         </is>
       </c>
     </row>
@@ -738,12 +808,17 @@
       </c>
       <c r="C15" s="3" t="inlineStr">
         <is>
-          <t>Mounts in an EIA-standard 19 in. Telco rack or equipment cabinet</t>
+          <t>1U</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
           <t>green</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Page 4</t>
         </is>
       </c>
     </row>
@@ -758,12 +833,17 @@
       </c>
       <c r="C16" s="3" t="inlineStr">
         <is>
-          <t>2-post rack kit included</t>
+          <t>Mounts in an EIA-standard 19 in. Telco rack or equipment cabinet.</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
           <t>green</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Page 28</t>
         </is>
       </c>
     </row>
@@ -786,6 +866,11 @@
           <t>green</t>
         </is>
       </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Page 25</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -798,12 +883,18 @@
       </c>
       <c r="C18" s="3" t="inlineStr">
         <is>
-          <t>2 field-replaceable, hot-swappable power supply slots</t>
+          <t>2 field-replaceable, hot-swappable power supply slots 
+1 minimum power supply required (ordered separately)</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
           <t>green</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Page 25</t>
         </is>
       </c>
     </row>
@@ -826,6 +917,11 @@
           <t>yellow</t>
         </is>
       </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -846,6 +942,11 @@
           <t>green</t>
         </is>
       </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Page 6</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -858,12 +959,17 @@
       </c>
       <c r="C21" s="3" t="inlineStr">
         <is>
-          <t>IEEE 802.1v protocol VLANs isolate select non-IPv4</t>
+          <t>IEEE 802.1v protocol VLANs</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
           <t>green</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Page 6</t>
         </is>
       </c>
     </row>
@@ -878,12 +984,17 @@
       </c>
       <c r="C22" s="3" t="inlineStr">
         <is>
-          <t>Bridge Protocol Data Unit (BPDU) tunneling transmits</t>
+          <t>Bridge Protocol Data Unit (BPDU) tunneling</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
           <t>green</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Page 6</t>
         </is>
       </c>
     </row>
@@ -898,12 +1009,19 @@
       </c>
       <c r="C23" s="3" t="inlineStr">
         <is>
-          <t>Jumbo packet support improves the performance of large data transfers; supports frame size of up to 9198 bytes</t>
+          <t>Jumbo packet support improves the performance 
+of large data transfers; supports frame size of up to 
+9198 bytes</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
           <t>green</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Page 6</t>
         </is>
       </c>
     </row>
@@ -918,12 +1036,19 @@
       </c>
       <c r="C24" s="3" t="inlineStr">
         <is>
-          <t>supports 4 mirroring groups</t>
+          <t>Port mirroring duplicates port traffic (ingress 
+and egress) to a monitoring port; supports 
+4 mirroring groups</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
           <t>green</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Page 6</t>
         </is>
       </c>
     </row>
@@ -946,6 +1071,11 @@
           <t>green</t>
         </is>
       </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Page 4</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -966,6 +1096,11 @@
           <t>green</t>
         </is>
       </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Page 6</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -978,12 +1113,18 @@
       </c>
       <c r="C27" s="3" t="inlineStr">
         <is>
-          <t>MVRP allows automatic learning and dynamic assignment of VLANs</t>
+          <t>MVRP allows automatic learning and dynamic 
+assignment of VLANs</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
           <t>green</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Page 6</t>
         </is>
       </c>
     </row>
@@ -1006,6 +1147,11 @@
           <t>green</t>
         </is>
       </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Page 5</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -1018,12 +1164,18 @@
       </c>
       <c r="C29" s="3" t="inlineStr">
         <is>
-          <t>LLDP-MED (Media Endpoint Discovery) defines a standard extension of LLDP</t>
+          <t>LLDP-MED (Media Endpoint Discovery) defines a 
+standard extension of LLDP</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
           <t>green</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Page 22</t>
         </is>
       </c>
     </row>
@@ -1046,6 +1198,11 @@
           <t>green</t>
         </is>
       </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Page 6</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -1066,6 +1223,11 @@
           <t>green</t>
         </is>
       </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Page 6</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -1078,12 +1240,18 @@
       </c>
       <c r="C32" s="3" t="inlineStr">
         <is>
-          <t>MVRP allows automatic learning and dynamic assignment of VLANs</t>
+          <t>MVRP allows automatic learning and dynamic 
+assignment of VLANs</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
           <t>green</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Page 6</t>
         </is>
       </c>
     </row>
@@ -1106,6 +1274,11 @@
           <t>green</t>
         </is>
       </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Page 6</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -1118,12 +1291,19 @@
       </c>
       <c r="C34" s="3" t="inlineStr">
         <is>
-          <t>VXLAN encapsulation tunneling protocol for overlay network</t>
+          <t>VXLAN encapsulation tunneling protocol for 
+overlay network that enables a more scalable virtual 
+network deployment</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
           <t>green</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Page 6</t>
         </is>
       </c>
     </row>
@@ -1146,6 +1326,11 @@
           <t>green</t>
         </is>
       </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Page 22</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
@@ -1158,12 +1343,17 @@
       </c>
       <c r="C36" s="3" t="inlineStr">
         <is>
-          <t>Static IP routing provides manually configured routing</t>
+          <t>Static IP routing</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
           <t>green</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Page 6</t>
         </is>
       </c>
     </row>
@@ -1186,6 +1376,11 @@
           <t>green</t>
         </is>
       </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Page 6</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -1198,12 +1393,17 @@
       </c>
       <c r="C38" s="3" t="inlineStr">
         <is>
-          <t>OSPF provides OSPFv2 for IPv4 routing and OSPFv3 for IPv6 routing</t>
+          <t>OSPFv3 for IPv6 routing</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
           <t>green</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Page 6</t>
         </is>
       </c>
     </row>
@@ -1218,12 +1418,17 @@
       </c>
       <c r="C39" s="3" t="inlineStr">
         <is>
-          <t>DHCP server centralizes and reduces the cost of IPv4 address management</t>
+          <t>DHCP server</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
           <t>green</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Page 6</t>
         </is>
       </c>
     </row>
@@ -1238,13 +1443,18 @@
       </c>
       <c r="C40" s="3" t="inlineStr">
         <is>
-          <t>2,048
+          <t>2,048 
 1,024</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
           <t>green</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Page 22</t>
         </is>
       </c>
     </row>
@@ -1259,12 +1469,17 @@
       </c>
       <c r="C41" s="3" t="inlineStr">
         <is>
-          <t>Packet storm protection against broadcast, multicast</t>
+          <t>Packet storm protection</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
           <t>green</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Page 4</t>
         </is>
       </c>
     </row>
@@ -1279,12 +1494,17 @@
       </c>
       <c r="C42" s="3" t="inlineStr">
         <is>
-          <t>ICMP throttling defeats ICMP denial-of-service attacks</t>
+          <t>ICMP throttling</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
           <t>green</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Page 7</t>
         </is>
       </c>
     </row>
@@ -1299,12 +1519,18 @@
       </c>
       <c r="C43" s="3" t="inlineStr">
         <is>
-          <t>Strict priority (SP) queuing and Deficit Weighted Round Robin (DWRR)</t>
+          <t>Strict priority (SP) queuing and Deficit Weighted
+Round Robin (DWRR)</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
           <t>green</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Page 5</t>
         </is>
       </c>
     </row>
@@ -1319,12 +1545,18 @@
       </c>
       <c r="C44" s="3" t="inlineStr">
         <is>
-          <t>Traffic prioritization (IEEE 802.1p) for real-time classification</t>
+          <t>Traffic prioritization (IEEE 802.1p) for
+real-time classification</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
           <t>green</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Page 5</t>
         </is>
       </c>
     </row>
@@ -1347,6 +1579,11 @@
           <t>green</t>
         </is>
       </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Page 5</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -1359,12 +1596,20 @@
       </c>
       <c r="C46" s="3" t="inlineStr">
         <is>
-          <t>Class of Service (CoS) sets the IEEE 802.1p priority tag based on IP address, IP Type of Service (ToS), Layer 3 protocol, TCP/UDP port number, source port, and DiffServ</t>
+          <t>Class of Service (CoS) sets the IEEE 802.1p priority 
+tag based on IP address, IP Type of Service (ToS), 
+Layer 3 protocol, TCP/UDP port number, source port,
+and DiffServ</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
           <t>green</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Page 5</t>
         </is>
       </c>
     </row>
@@ -1387,6 +1632,11 @@
           <t>yellow</t>
         </is>
       </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
@@ -1399,12 +1649,18 @@
       </c>
       <c r="C48" s="3" t="inlineStr">
         <is>
-          <t>Access control list (ACL) support for both IPv4 and IPv6</t>
+          <t>Access control list (ACL) support for both IPv4 and
+IPv6</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
           <t>green</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Page 7</t>
         </is>
       </c>
     </row>
@@ -1419,12 +1675,20 @@
       </c>
       <c r="C49" s="3" t="inlineStr">
         <is>
-          <t>ACLs also provide filtering based on the IP field, source/destination IP address/subnet, and source/destination TCP/UDP port number on a per-VLAN or per-port basis</t>
+          <t>ACLs also provide filtering based on the IP field, 
+source/destination IP address/subnet, and 
+source/destination TCP/UDP port number on a 
+per-VLAN or per-port basis</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
           <t>green</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Page 7</t>
         </is>
       </c>
     </row>
@@ -1439,12 +1703,17 @@
       </c>
       <c r="C50" s="3" t="inlineStr">
         <is>
-          <t>The HPE Aruba Networking Dynamic Segmentation solution enables seamless mobility, consistent policy enforcement, and automated configurations for wired and wireless clients across networks of all sizes. It unifies role-based access and policy enforcement across LAN, WLAN</t>
+          <t>Role-based microsegmentation</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
           <t>green</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Page 3</t>
         </is>
       </c>
     </row>
@@ -1459,12 +1728,18 @@
       </c>
       <c r="C51" s="3" t="inlineStr">
         <is>
-          <t>Uses an IEEE 802.1X supplicant</t>
+          <t>Uses 
+an IEEE 802.1X supplicant on the client</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
           <t>green</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Page 7</t>
         </is>
       </c>
     </row>
@@ -1487,6 +1762,11 @@
           <t>green</t>
         </is>
       </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Page 7</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
@@ -1507,6 +1787,11 @@
           <t>green</t>
         </is>
       </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Page 7</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
@@ -1519,12 +1804,19 @@
       </c>
       <c r="C54" s="3" t="inlineStr">
         <is>
-          <t>Concurrent IEEE 802.1X, Web, and MAC authentication schemes per switch port accepts up to 32 sessions of IEEE 802.1X, Web, and MAC authentications</t>
+          <t>Concurrent IEEE 802.1X, Web, and MAC authentication 
+schemes per switch port accepts up to 32 sessions of 
+IEEE 802.1X, Web, and MAC authentications</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
           <t>green</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Page 7</t>
         </is>
       </c>
     </row>
@@ -1539,12 +1831,18 @@
       </c>
       <c r="C55" s="3" t="inlineStr">
         <is>
-          <t>Terminal Access Controller Access-Control System (TACACS+)</t>
+          <t>Terminal Access Controller Access-Control System
+(TACACS+)</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
           <t>green</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Page 7</t>
         </is>
       </c>
     </row>
@@ -1559,12 +1857,19 @@
       </c>
       <c r="C56" s="3" t="inlineStr">
         <is>
-          <t>Switch CPU protection provides automatic protection against malicious network traffic trying to shut down the switch</t>
+          <t>Switch CPU protection provides automatic protection
+against malicious network traffic trying to shut down
+the switch</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
           <t>green</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Page 7</t>
         </is>
       </c>
     </row>
@@ -1587,6 +1892,11 @@
           <t>green</t>
         </is>
       </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Page 5</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
@@ -1599,12 +1909,19 @@
       </c>
       <c r="C58" s="3" t="inlineStr">
         <is>
-          <t>Dual flash images provides independent primary and secondary operating system files for backup while upgrading</t>
+          <t>Dual flash images provides independent primary
+and secondary operating system files for backup
+while upgrading</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
           <t>green</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Page 5</t>
         </is>
       </c>
     </row>
@@ -1619,12 +1936,18 @@
       </c>
       <c r="C59" s="3" t="inlineStr">
         <is>
-          <t>Multiple configuration files can be stored to a flash image</t>
+          <t>Multiple configuration files can be stored to a
+flash image</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
           <t>green</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>Page 5</t>
         </is>
       </c>
     </row>
@@ -1647,6 +1970,11 @@
           <t>yellow</t>
         </is>
       </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -1659,12 +1987,18 @@
       </c>
       <c r="C61" s="3" t="inlineStr">
         <is>
-          <t>Unidirectional link detection (UDLD)</t>
+          <t>Ingress and egress port monitoring enable more
+efficient network problem solving</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
           <t>green</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>Page 5</t>
         </is>
       </c>
     </row>
@@ -1679,12 +2013,17 @@
       </c>
       <c r="C62" s="3" t="inlineStr">
         <is>
-          <t>sFlow® (RFC 3176) is ASIC-based wire speed network monitoring and accounting</t>
+          <t>sFlow® (RFC 3176)</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
           <t>green</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>Page 5</t>
         </is>
       </c>
     </row>
@@ -1699,12 +2038,18 @@
       </c>
       <c r="C63" s="3" t="inlineStr">
         <is>
-          <t>allowing secure access to the browser-based management GUI in the switch</t>
+          <t>allowing secure access to the browser-based 
+management GUI in the switch</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
           <t>green</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>Page 7</t>
         </is>
       </c>
     </row>
@@ -1719,12 +2064,18 @@
       </c>
       <c r="C64" s="3" t="inlineStr">
         <is>
-          <t>local and remote syslog capabilities allow logging of all access</t>
+          <t>local and remote
+syslog capabilities</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
           <t>green</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>Page 5</t>
         </is>
       </c>
     </row>
@@ -1739,12 +2090,17 @@
       </c>
       <c r="C65" s="3" t="inlineStr">
         <is>
-          <t>Secure FTP allows secure file transfer to and from the switch</t>
+          <t>Secure File Transfer Protocol (SFTP)</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
           <t>green</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>Page 5</t>
         </is>
       </c>
     </row>
@@ -1759,12 +2115,17 @@
       </c>
       <c r="C66" s="3" t="inlineStr">
         <is>
-          <t>SNMPv1/v2c/v3</t>
+          <t>Supports SNMP (v2c/v3)</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
           <t>green</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>Page 5</t>
         </is>
       </c>
     </row>
@@ -1787,6 +2148,11 @@
           <t>green</t>
         </is>
       </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>Page 8</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
@@ -1799,12 +2165,19 @@
       </c>
       <c r="C68" s="3" t="inlineStr">
         <is>
-          <t>An easy-to-use mobile app simplifies connecting, stacking and managing HPE Aruba Networking CX 6200 switches for any size project.</t>
+          <t>An easy-to-use mobile app simplifies connecting, 
+stacking and managing HPE Aruba Networking CX 
+6200 switches for any size project.</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
           <t>green</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>Page 3</t>
         </is>
       </c>
     </row>
@@ -1817,14 +2190,22 @@
           <t>Deve suportar o encaminhamento de tráfego para gateway do mesmo fabricante para inspeção e controle de acesso;</t>
         </is>
       </c>
-      <c r="C69" s="2" t="inlineStr">
-        <is>
-          <t>None</t>
+      <c r="C69" s="3" t="inlineStr">
+        <is>
+          <t>Dynamic Segmentation provides scale and flexibility in 
+network design by allowing the stretching of VLANs and 
+subnets across the entire network with a VXLAN-based 
+distributed overlay fabric.</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>yellow</t>
+          <t>green</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>Page 3</t>
         </is>
       </c>
     </row>

</xml_diff>